<commit_message>
Es04: Misure & screen invamp, ALPF
</commit_message>
<xml_diff>
--- a/Es04/data/opamp_gain.xlsx
+++ b/Es04/data/opamp_gain.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berni\Desktop\Lab3\Es04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berni\Desktop\Lab3\Es04\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C9BE13-DD01-48CF-BA0F-21B571DE16C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B225B5-2546-4852-98BE-84C3A3AFF9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5055" yWindow="6465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>500 medie</t>
   </si>
@@ -62,11 +62,20 @@
   <si>
     <t>txt</t>
   </si>
+  <si>
+    <t>Av</t>
+  </si>
+  <si>
+    <t>sigma_Av</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -387,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +415,7 @@
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -430,8 +440,23 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40.1</v>
       </c>
@@ -452,8 +477,36 @@
         <f>SQRT((C2*5/1000)^2 + (0.1/SQRT(12)*D2)^2)</f>
         <v>1.6589831222770171</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>C2/A2</f>
+        <v>7.0573566084788029</v>
+      </c>
+      <c r="J2">
+        <f>I2*SQRT((G2/A2)^2 + (H2/C2)^2)</f>
+        <v>5.8049237479244536E-2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>0.4</v>
+      </c>
+      <c r="O2">
+        <v>256</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <f>O2/M2</f>
+        <v>5.12</v>
+      </c>
+      <c r="R2">
+        <f>Q2*SQRT((N2/M2)^2 + (P2/O2)^2)</f>
+        <v>5.7251389502788491E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59.8</v>
       </c>
@@ -474,8 +527,36 @@
         <f t="shared" ref="H3:H11" si="1">SQRT((C3*5/1000)^2 + (0.1/SQRT(12)*D3)^2)</f>
         <v>2.5071564237863848</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="2">C3/A3</f>
+        <v>6.8561872909699</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J11" si="3">I3*SQRT((G3/A3)^2 + (H3/C3)^2)</f>
+        <v>5.7682739884246513E-2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>0.8</v>
+      </c>
+      <c r="O3">
+        <v>511</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q13" si="4">O3/M3</f>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R13" si="5">Q3*SQRT((N3/M3)^2 + (P3/O3)^2)</f>
+        <v>5.7194181522249275E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>79.900000000000006</v>
       </c>
@@ -496,8 +577,36 @@
         <f t="shared" si="1"/>
         <v>3.3094410404175503</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>7.0588235294117645</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>5.8116593863514331E-2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>150</v>
+      </c>
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+      <c r="O4">
+        <v>767</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="4"/>
+        <v>5.1133333333333333</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="5"/>
+        <v>5.7213244775818982E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100.1</v>
       </c>
@@ -518,8 +627,36 @@
         <f t="shared" si="1"/>
         <v>4.1368013005219382</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>7.0429570429570436</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>5.7969914468023631E-2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>200</v>
+      </c>
+      <c r="N5">
+        <v>1.6</v>
+      </c>
+      <c r="O5">
+        <v>1022</v>
+      </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="4"/>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="5"/>
+        <v>5.7194181522249275E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -540,8 +677,36 @@
         <f t="shared" si="1"/>
         <v>8.2821253310970846</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>7.06</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>5.8105880367939816E-2</v>
+      </c>
+      <c r="M6">
+        <v>250</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>1278</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="4"/>
+        <v>5.1120000000000001</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="5"/>
+        <v>6.0070648539865129E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>401</v>
       </c>
@@ -562,8 +727,36 @@
         <f t="shared" si="1"/>
         <v>16.55572710574803</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>7.0374064837905239</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>5.7907881686432225E-2</v>
+      </c>
+      <c r="M7">
+        <v>300</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>1534</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="4"/>
+        <v>5.1133333333333333</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="5"/>
+        <v>5.25552313826037E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>601</v>
       </c>
@@ -584,8 +777,36 @@
         <f t="shared" si="1"/>
         <v>24.842113939840143</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>7.0465890183028286</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>5.7985542983223455E-2</v>
+      </c>
+      <c r="M8">
+        <v>349</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>1790</v>
+      </c>
+      <c r="P8">
+        <v>14</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="4"/>
+        <v>5.1289398280802292</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="5"/>
+        <v>5.9606720182919341E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>801</v>
       </c>
@@ -606,8 +827,36 @@
         <f t="shared" si="1"/>
         <v>33.671436337049833</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>7.2097378277153554</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>5.9149680718866372E-2</v>
+      </c>
+      <c r="M9">
+        <v>399</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>2046</v>
+      </c>
+      <c r="P9">
+        <v>16</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>5.1278195488721803</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="5"/>
+        <v>5.562841686255697E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>902</v>
       </c>
@@ -628,8 +877,36 @@
         <f t="shared" si="1"/>
         <v>38.293109367091105</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>7.0033259423503322</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>5.9420771999761195E-2</v>
+      </c>
+      <c r="M10">
+        <v>449</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>2302</v>
+      </c>
+      <c r="P10">
+        <v>18</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="4"/>
+        <v>5.1269487750556797</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="5"/>
+        <v>6.0772391465453532E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1002</v>
       </c>
@@ -650,8 +927,80 @@
         <f t="shared" si="1"/>
         <v>41.312640014891329</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>7.0229540918163673</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>5.7813072713296866E-2</v>
+      </c>
+      <c r="M11">
+        <v>499</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>2558</v>
+      </c>
+      <c r="P11">
+        <v>20</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="4"/>
+        <v>5.1262525050100196</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="5"/>
+        <v>5.74019905386993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>549</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>2815</v>
+      </c>
+      <c r="P12">
+        <v>22</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="4"/>
+        <v>5.1275045537340622</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="5"/>
+        <v>5.478612108218131E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>599</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>3073</v>
+      </c>
+      <c r="P13">
+        <v>24</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>5.1302170283806348</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="5"/>
+        <v>5.8644449760373613E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -659,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>40.1</v>
       </c>
@@ -673,7 +1022,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>59.8</v>
       </c>

</xml_diff>

<commit_message>
Es04: saturazione invertente; pinna di squalo
</commit_message>
<xml_diff>
--- a/Es04/data/opamp_gain.xlsx
+++ b/Es04/data/opamp_gain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berni\Desktop\Lab3\Es04\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B225B5-2546-4852-98BE-84C3A3AFF9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20E9131-4164-440B-9F4B-F6276406BAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="6465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5700" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +86,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,10 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -399,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,11 +557,11 @@
         <v>4</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q13" si="4">O3/M3</f>
+        <f t="shared" ref="Q3:Q22" si="4">O3/M3</f>
         <v>5.1100000000000003</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R13" si="5">Q3*SQRT((N3/M3)^2 + (P3/O3)^2)</f>
+        <f t="shared" ref="R3:R22" si="5">Q3*SQRT((N3/M3)^2 + (P3/O3)^2)</f>
         <v>5.7194181522249275E-2</v>
       </c>
     </row>
@@ -1007,6 +1016,26 @@
       <c r="B14" t="s">
         <v>8</v>
       </c>
+      <c r="M14">
+        <v>699</v>
+      </c>
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>3546</v>
+      </c>
+      <c r="P14">
+        <v>30</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>5.0729613733905579</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="5"/>
+        <v>6.1140310191574829E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1021,6 +1050,26 @@
       <c r="D15">
         <v>1.7</v>
       </c>
+      <c r="M15">
+        <v>799</v>
+      </c>
+      <c r="N15">
+        <v>6</v>
+      </c>
+      <c r="O15">
+        <v>3819</v>
+      </c>
+      <c r="P15">
+        <v>31</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="4"/>
+        <v>4.7797246558197743</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="5"/>
+        <v>5.285467448052053E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1035,8 +1084,28 @@
       <c r="D16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>899</v>
+      </c>
+      <c r="N16">
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <v>3845</v>
+      </c>
+      <c r="P16">
+        <v>32</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>4.2769744160177972</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="5"/>
+        <v>4.8744832295464738E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>79.900000000000006</v>
       </c>
@@ -1049,8 +1118,28 @@
       <c r="D17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>999</v>
+      </c>
+      <c r="N17">
+        <v>8</v>
+      </c>
+      <c r="O17">
+        <v>3860</v>
+      </c>
+      <c r="P17">
+        <v>32</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="4"/>
+        <v>3.8638638638638638</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="5"/>
+        <v>4.4535933004148938E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>100.1</v>
       </c>
@@ -1063,8 +1152,28 @@
       <c r="D18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>1199</v>
+      </c>
+      <c r="N18">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>3855</v>
+      </c>
+      <c r="P18">
+        <v>32</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="4"/>
+        <v>3.2151793160967475</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="5"/>
+        <v>3.5982574057794391E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>200</v>
       </c>
@@ -1077,8 +1186,28 @@
       <c r="D19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1399</v>
+      </c>
+      <c r="N19">
+        <v>11</v>
+      </c>
+      <c r="O19">
+        <v>3883</v>
+      </c>
+      <c r="P19">
+        <v>32</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="4"/>
+        <v>2.7755539671193712</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="5"/>
+        <v>3.1614266125429974E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>401</v>
       </c>
@@ -1091,8 +1220,28 @@
       <c r="D20">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>1599</v>
+      </c>
+      <c r="N20">
+        <v>12</v>
+      </c>
+      <c r="O20">
+        <v>3890</v>
+      </c>
+      <c r="P20">
+        <v>32</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="4"/>
+        <v>2.4327704815509694</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="5"/>
+        <v>2.7089212470732583E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>601</v>
       </c>
@@ -1105,8 +1254,28 @@
       <c r="D21">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>1799</v>
+      </c>
+      <c r="N21">
+        <v>14</v>
+      </c>
+      <c r="O21">
+        <v>3906</v>
+      </c>
+      <c r="P21">
+        <v>32</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="4"/>
+        <v>2.1712062256809337</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="5"/>
+        <v>2.4533530632423695E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>801</v>
       </c>
@@ -1119,8 +1288,28 @@
       <c r="D22">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>1999</v>
+      </c>
+      <c r="N22">
+        <v>15</v>
+      </c>
+      <c r="O22">
+        <v>3921</v>
+      </c>
+      <c r="P22">
+        <v>32</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="4"/>
+        <v>1.961480740370185</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="5"/>
+        <v>2.1746020274071739E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>902</v>
       </c>
@@ -1133,8 +1322,16 @@
       <c r="D23">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="O23" s="3">
+        <f>AVERAGE(O16:O22)</f>
+        <v>3880</v>
+      </c>
+      <c r="P23">
+        <f>STDEV(O16:O22)</f>
+        <v>28.035691537752374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1002</v>
       </c>

</xml_diff>